<commit_message>
Conditional distributions section now complete.
</commit_message>
<xml_diff>
--- a/Intro_coinBiased.xlsx
+++ b/Intro_coinBiased.xlsx
@@ -16,22 +16,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Coin A</t>
   </si>
   <si>
     <t>Coin B</t>
   </si>
+  <si>
+    <t>p(X_B|X_A=1)</t>
+  </si>
+  <si>
+    <t>p(X_A)</t>
+  </si>
+  <si>
+    <t>"=0.1/0.6 = 1/6"</t>
+  </si>
+  <si>
+    <t>"=0.5/0.6 = 5/6"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -65,19 +84,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -383,10 +405,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
@@ -401,6 +426,9 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -412,12 +440,11 @@
       <c r="C3" s="1">
         <v>0.3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>0.1</v>
       </c>
-      <c r="E3" s="2">
-        <f>SUM(C3:D3)</f>
-        <v>0.4</v>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -428,15 +455,17 @@
       <c r="C4" s="1">
         <v>0.1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>0.5</v>
       </c>
-      <c r="E4" s="2">
-        <f>SUM(C4:D4)</f>
-        <v>0.6</v>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C5" s="2">
         <f>SUM(C3:C4)</f>
         <v>0.4</v>

</xml_diff>